<commit_message>
Add enough data to the insecurity test data that we can bin it. Remove the separate file that I had intended to bin on it's own because everything has to go through the same function that will try to calculate bins and fail if there isn't enough data
</commit_message>
<xml_diff>
--- a/tests/resources/insecurity/test_food_insecurity_xlsx.xlsx
+++ b/tests/resources/insecurity/test_food_insecurity_xlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t xml:space="preserve">Version/Updates</t>
   </si>
@@ -110,6 +110,18 @@
   </si>
   <si>
     <t xml:space="preserve">Jo Daviess County, Illinois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Johnson County, Illinois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kane County, Illinois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kankakee County, Illinois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kendall County, Illinois</t>
   </si>
 </sst>
 </file>
@@ -215,7 +227,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -237,19 +249,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -344,7 +352,7 @@
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="71.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.1"/>
@@ -416,7 +424,7 @@
       <c r="D6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -450,21 +458,21 @@
       <c r="D8" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="5"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="5"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
@@ -500,55 +508,123 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="5" width="29.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="44.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="44.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="39.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="50.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="5" width="8.89"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+    <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>0.09</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="8" t="n">
         <v>0.133</v>
       </c>
-      <c r="D2" s="10" t="n">
+      <c r="D2" s="9" t="n">
         <v>0.128</v>
       </c>
-      <c r="E2" s="9" t="n">
+      <c r="E2" s="8" t="n">
         <v>0.212</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>0.119</v>
+      </c>
+      <c r="C3" s="8" t="n">
+        <v>0.163</v>
+      </c>
+      <c r="D3" s="9" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="E3" s="8" t="n">
+        <v>0.268</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>0.071</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="D4" s="9" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <v>0.183</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="C5" s="8" t="n">
+        <v>0.157</v>
+      </c>
+      <c r="D5" s="9" t="n">
+        <v>0.157</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>0.238</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>0.092</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="E6" s="8" t="n">
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Bins for Food Insecurity Data (#61)
* Add failing test for bins

* Add enough data to the insecurity test data that we can bin it. Remove the separate file that I had intended to bin on it's own because everything has to go through the same function that will try to calculate bins and fail if there isn't enough data

* Add quantiles bins

* Add tests to verify the bins are present for all the insecurity fields because it isn't that hard to add

* Fix flake8 errors

* Nest the insecurity bins under a 'insecurity_data' object so the bins match the metrics per county

* Update the expected output of the file_to_json test. I had forgotten that this uses the same input as the food insecurity test
</commit_message>
<xml_diff>
--- a/tests/resources/insecurity/test_food_insecurity_xlsx.xlsx
+++ b/tests/resources/insecurity/test_food_insecurity_xlsx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t xml:space="preserve">Version/Updates</t>
   </si>
@@ -110,6 +110,18 @@
   </si>
   <si>
     <t xml:space="preserve">Jo Daviess County, Illinois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Johnson County, Illinois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kane County, Illinois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kankakee County, Illinois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kendall County, Illinois</t>
   </si>
 </sst>
 </file>
@@ -215,7 +227,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -237,19 +249,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -344,7 +352,7 @@
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="71.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.1"/>
@@ -416,7 +424,7 @@
       <c r="D6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -450,21 +458,21 @@
       <c r="D8" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="5"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="5"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
@@ -500,55 +508,123 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="5" width="29.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="44.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="44.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="39.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="50.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="5" width="8.89"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+    <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>0.09</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="8" t="n">
         <v>0.133</v>
       </c>
-      <c r="D2" s="10" t="n">
+      <c r="D2" s="9" t="n">
         <v>0.128</v>
       </c>
-      <c r="E2" s="9" t="n">
+      <c r="E2" s="8" t="n">
         <v>0.212</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>0.119</v>
+      </c>
+      <c r="C3" s="8" t="n">
+        <v>0.163</v>
+      </c>
+      <c r="D3" s="9" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="E3" s="8" t="n">
+        <v>0.268</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>0.071</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="D4" s="9" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <v>0.183</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="C5" s="8" t="n">
+        <v>0.157</v>
+      </c>
+      <c r="D5" s="9" t="n">
+        <v>0.157</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>0.238</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>0.092</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="E6" s="8" t="n">
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>